<commit_message>
import xlsx working w/bug
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yerson Quiroz\Repositorios Git\RedSalud\RedSalud-DIRSAL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1B862EBC-5B78-4988-AF00-421BEE070258}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{366F39AD-2B5C-4E6A-A143-AD36F2F9815B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{9E8E4BC8-A1CC-4D91-A4B0-E08C2B0290A8}"/>
+    <workbookView xWindow="9576" yWindow="4200" windowWidth="17280" windowHeight="8964" xr2:uid="{9E8E4BC8-A1CC-4D91-A4B0-E08C2B0290A8}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -30,21 +30,84 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="26">
   <si>
     <t>hola</t>
   </si>
   <si>
-    <t>asdasd</t>
-  </si>
-  <si>
-    <t>ing</t>
-  </si>
-  <si>
-    <t>de</t>
-  </si>
-  <si>
-    <t>soft</t>
+    <t>rut</t>
+  </si>
+  <si>
+    <t>nombre</t>
+  </si>
+  <si>
+    <t>estado</t>
+  </si>
+  <si>
+    <t>activo</t>
+  </si>
+  <si>
+    <t>inactivo</t>
+  </si>
+  <si>
+    <t>prevision</t>
+  </si>
+  <si>
+    <t>fonasa</t>
+  </si>
+  <si>
+    <t>isapre</t>
+  </si>
+  <si>
+    <t>yerso</t>
+  </si>
+  <si>
+    <t>thomas</t>
+  </si>
+  <si>
+    <t>leandro</t>
+  </si>
+  <si>
+    <t>perkinazo</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>ctm</t>
+  </si>
+  <si>
+    <t>asd</t>
+  </si>
+  <si>
+    <t>afiliado</t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t>false</t>
+  </si>
+  <si>
+    <t>jorsi</t>
+  </si>
+  <si>
+    <t>yapo</t>
+  </si>
+  <si>
+    <t>8237478-9</t>
+  </si>
+  <si>
+    <t>culi</t>
+  </si>
+  <si>
+    <t>nelson</t>
+  </si>
+  <si>
+    <t>genial</t>
+  </si>
+  <si>
+    <t>bueno</t>
   </si>
 </sst>
 </file>
@@ -396,55 +459,156 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C573FF0-013F-4B94-83DE-64E889252B94}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1">
-        <v>123</v>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>1</v>
       </c>
       <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>82937288</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
         <v>0</v>
       </c>
+      <c r="F2" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>34</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1</v>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" t="s">
+        <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>45246</v>
-      </c>
-      <c r="B3" t="s">
-        <v>2</v>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>1248238</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" t="s">
+        <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>532</v>
-      </c>
-      <c r="B4" t="s">
-        <v>3</v>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>23743728</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" t="s">
+        <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>425</v>
-      </c>
-      <c r="B5" t="s">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>4357984</v>
+      </c>
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>12345678</v>
+      </c>
+      <c r="B7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" t="s">
         <v>4</v>
+      </c>
+      <c r="D7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
remove solicitud working, minor changes
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yerson Quiroz\Repositorios Git\RedSalud\RedSalud-DIRSAL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49AF9055-1198-48D5-BF7B-3EA65DD809A5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4553B14D-9B93-46A2-8378-6A4C49E382A2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2916" yWindow="2964" windowWidth="17280" windowHeight="8964" xr2:uid="{9E8E4BC8-A1CC-4D91-A4B0-E08C2B0290A8}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
   <si>
     <t>rut</t>
   </si>
@@ -62,18 +62,9 @@
     <t>leandro</t>
   </si>
   <si>
-    <t>perkinazo</t>
-  </si>
-  <si>
     <t>email</t>
   </si>
   <si>
-    <t>ctm</t>
-  </si>
-  <si>
-    <t>asd</t>
-  </si>
-  <si>
     <t>afiliado</t>
   </si>
   <si>
@@ -86,30 +77,46 @@
     <t>jorsi</t>
   </si>
   <si>
-    <t>yapo</t>
-  </si>
-  <si>
     <t>8237478-9</t>
   </si>
   <si>
-    <t>culi</t>
-  </si>
-  <si>
-    <t>nelson</t>
-  </si>
-  <si>
-    <t>genial</t>
-  </si>
-  <si>
-    <t>bueno</t>
+    <t>thomas@redsalud.dirsal</t>
+  </si>
+  <si>
+    <t>leandro@redsalud.dirsal</t>
+  </si>
+  <si>
+    <t>jorsi@redsalud.dirsal</t>
+  </si>
+  <si>
+    <t>pretoriano</t>
+  </si>
+  <si>
+    <t>pretorian@mail</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -134,13 +141,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -456,7 +467,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -475,15 +486,15 @@
         <v>5</v>
       </c>
       <c r="E1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" t="s">
         <v>11</v>
-      </c>
-      <c r="F1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
@@ -494,11 +505,11 @@
       <c r="D2" t="s">
         <v>7</v>
       </c>
-      <c r="E2" t="s">
-        <v>20</v>
+      <c r="E2" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="F2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -514,11 +525,11 @@
       <c r="D3" t="s">
         <v>7</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" t="s">
         <v>12</v>
-      </c>
-      <c r="F3" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -526,7 +537,7 @@
         <v>23743728</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C4" t="s">
         <v>4</v>
@@ -534,55 +545,49 @@
       <c r="D4" t="s">
         <v>6</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" t="s">
         <v>13</v>
-      </c>
-      <c r="F4" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>4357984</v>
-      </c>
-      <c r="B5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="A5" s="2">
+        <v>12345678</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F5" t="s">
-        <v>15</v>
+      <c r="E5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>12345678</v>
-      </c>
-      <c r="B6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D6" t="s">
-        <v>22</v>
-      </c>
-      <c r="E6" t="s">
-        <v>23</v>
-      </c>
-      <c r="F6" t="s">
-        <v>16</v>
-      </c>
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{3CA5C219-936F-403B-AA11-A98DF9641EBE}"/>
+    <hyperlink ref="E3" r:id="rId2" xr:uid="{04952068-CD8A-4210-AA5C-9CE08A761B29}"/>
+    <hyperlink ref="E4" r:id="rId3" xr:uid="{72D50ACE-DAF0-4ED6-B647-1666FAC81A08}"/>
+    <hyperlink ref="E5" r:id="rId4" xr:uid="{B71DEF31-F6E3-4666-BD89-5FC11422DAFA}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>